<commit_message>
added analyze with collocations & selector of dictionary (files analyzer) & tests
</commit_message>
<xml_diff>
--- a/app/static/test.xlsx
+++ b/app/static/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\sentiment-analyzer\app\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEE8EF0-DE97-43E2-B372-AE5F2C57CEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCDD207-CF8A-456E-AA6D-9AAB34687560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D3F589C-E8BE-47A3-AB9E-FE283CEFC3F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Достоинств много, но почти все их можно увидеть в характеристиках.
 1) работу с двумя симками, но мне это было не надо)
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>очень хороший телефон, мне безумно понравился</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7864E01D-0914-4F84-95AB-93A5A7091137}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,49 +511,54 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>